<commit_message>
se creó validación 13 que permite entrenar mejor los modelos
</commit_message>
<xml_diff>
--- a/datosCobre.xlsx
+++ b/datosCobre.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="1183">
   <si>
     <t>fecha</t>
   </si>
@@ -22,15 +22,6 @@
     <t>valor</t>
   </si>
   <si>
-    <t>2022-04-03</t>
-  </si>
-  <si>
-    <t>2022-04-04</t>
-  </si>
-  <si>
-    <t>2022-04-05</t>
-  </si>
-  <si>
     <t>2022-04-06</t>
   </si>
   <si>
@@ -2215,10 +2206,13 @@
     <t>2024-04-02</t>
   </si>
   <si>
-    <t>467.27</t>
-  </si>
-  <si>
-    <t>472.92</t>
+    <t>2024-04-03</t>
+  </si>
+  <si>
+    <t>2024-04-04</t>
+  </si>
+  <si>
+    <t>2024-04-05</t>
   </si>
   <si>
     <t>469.49</t>
@@ -3563,6 +3557,12 @@
   </si>
   <si>
     <t>394.44</t>
+  </si>
+  <si>
+    <t>404.60</t>
+  </si>
+  <si>
+    <t>405.15</t>
   </si>
 </sst>
 </file>
@@ -3941,6 +3941,9 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
@@ -3950,7 +3953,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3961,7 +3964,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3983,7 +3986,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3994,7 +3997,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4016,7 +4019,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4027,7 +4030,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4049,7 +4052,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4060,7 +4063,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4071,7 +4074,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4082,7 +4085,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4104,7 +4107,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4115,7 +4118,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4137,7 +4140,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -4148,7 +4151,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4170,7 +4173,7 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4181,7 +4184,7 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -4192,7 +4195,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4214,7 +4217,7 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -4225,7 +4228,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -4236,7 +4239,7 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4258,7 +4261,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4269,7 +4272,7 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4291,7 +4294,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4302,7 +4305,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -4324,7 +4327,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -4335,7 +4338,7 @@
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -4346,7 +4349,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -4368,7 +4371,7 @@
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -4379,7 +4382,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -4401,7 +4404,7 @@
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -4412,7 +4415,7 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -4423,7 +4426,7 @@
         <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -4445,7 +4448,7 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4456,7 +4459,7 @@
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4478,7 +4481,7 @@
         <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -4511,7 +4514,7 @@
         <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -4522,7 +4525,7 @@
         <v>55</v>
       </c>
       <c r="C55" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -4533,7 +4536,7 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -4544,7 +4547,7 @@
         <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -4566,7 +4569,7 @@
         <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -4577,7 +4580,7 @@
         <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -4588,7 +4591,7 @@
         <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -4599,7 +4602,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -4610,7 +4613,7 @@
         <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -4632,7 +4635,7 @@
         <v>65</v>
       </c>
       <c r="C65" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -4643,7 +4646,7 @@
         <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -4654,7 +4657,7 @@
         <v>67</v>
       </c>
       <c r="C67" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -4676,7 +4679,7 @@
         <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -4687,7 +4690,7 @@
         <v>70</v>
       </c>
       <c r="C70" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -4709,7 +4712,7 @@
         <v>72</v>
       </c>
       <c r="C72" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -4720,7 +4723,7 @@
         <v>73</v>
       </c>
       <c r="C73" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -4731,7 +4734,7 @@
         <v>74</v>
       </c>
       <c r="C74" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -4753,7 +4756,7 @@
         <v>76</v>
       </c>
       <c r="C76" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -4764,7 +4767,7 @@
         <v>77</v>
       </c>
       <c r="C77" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -4786,7 +4789,7 @@
         <v>79</v>
       </c>
       <c r="C79" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -4797,7 +4800,7 @@
         <v>80</v>
       </c>
       <c r="C80" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -4808,7 +4811,7 @@
         <v>81</v>
       </c>
       <c r="C81" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -4830,7 +4833,7 @@
         <v>83</v>
       </c>
       <c r="C83" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -4841,7 +4844,7 @@
         <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -4863,7 +4866,7 @@
         <v>86</v>
       </c>
       <c r="C86" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -4874,7 +4877,7 @@
         <v>87</v>
       </c>
       <c r="C87" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -4885,7 +4888,7 @@
         <v>88</v>
       </c>
       <c r="C88" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -4907,7 +4910,7 @@
         <v>90</v>
       </c>
       <c r="C90" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -4918,7 +4921,7 @@
         <v>91</v>
       </c>
       <c r="C91" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -4940,7 +4943,7 @@
         <v>93</v>
       </c>
       <c r="C93" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -4951,7 +4954,7 @@
         <v>94</v>
       </c>
       <c r="C94" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -4962,7 +4965,7 @@
         <v>95</v>
       </c>
       <c r="C95" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -4984,7 +4987,7 @@
         <v>97</v>
       </c>
       <c r="C97" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -4995,7 +4998,7 @@
         <v>98</v>
       </c>
       <c r="C98" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -5017,7 +5020,7 @@
         <v>100</v>
       </c>
       <c r="C100" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -5028,7 +5031,7 @@
         <v>101</v>
       </c>
       <c r="C101" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -5039,7 +5042,7 @@
         <v>102</v>
       </c>
       <c r="C102" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -5061,7 +5064,7 @@
         <v>104</v>
       </c>
       <c r="C104" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -5072,7 +5075,7 @@
         <v>105</v>
       </c>
       <c r="C105" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -5094,7 +5097,7 @@
         <v>107</v>
       </c>
       <c r="C107" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -5105,7 +5108,7 @@
         <v>108</v>
       </c>
       <c r="C108" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -5116,7 +5119,7 @@
         <v>109</v>
       </c>
       <c r="C109" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -5138,7 +5141,7 @@
         <v>111</v>
       </c>
       <c r="C111" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -5149,7 +5152,7 @@
         <v>112</v>
       </c>
       <c r="C112" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -5171,7 +5174,7 @@
         <v>114</v>
       </c>
       <c r="C114" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -5182,7 +5185,7 @@
         <v>115</v>
       </c>
       <c r="C115" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -5193,7 +5196,7 @@
         <v>116</v>
       </c>
       <c r="C116" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -5215,7 +5218,7 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -5226,7 +5229,7 @@
         <v>119</v>
       </c>
       <c r="C119" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -5248,7 +5251,7 @@
         <v>121</v>
       </c>
       <c r="C121" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -5259,7 +5262,7 @@
         <v>122</v>
       </c>
       <c r="C122" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -5270,7 +5273,7 @@
         <v>123</v>
       </c>
       <c r="C123" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -5292,7 +5295,7 @@
         <v>125</v>
       </c>
       <c r="C125" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -5303,7 +5306,7 @@
         <v>126</v>
       </c>
       <c r="C126" t="s">
-        <v>815</v>
+        <v>792</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -5314,7 +5317,7 @@
         <v>127</v>
       </c>
       <c r="C127" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -5336,7 +5339,7 @@
         <v>129</v>
       </c>
       <c r="C129" t="s">
-        <v>794</v>
+        <v>816</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -5347,7 +5350,7 @@
         <v>130</v>
       </c>
       <c r="C130" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -5369,7 +5372,7 @@
         <v>132</v>
       </c>
       <c r="C132" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -5380,7 +5383,7 @@
         <v>133</v>
       </c>
       <c r="C133" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -5402,7 +5405,7 @@
         <v>135</v>
       </c>
       <c r="C135" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -5413,7 +5416,7 @@
         <v>136</v>
       </c>
       <c r="C136" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -5424,7 +5427,7 @@
         <v>137</v>
       </c>
       <c r="C137" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -5446,7 +5449,7 @@
         <v>139</v>
       </c>
       <c r="C139" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -5457,7 +5460,7 @@
         <v>140</v>
       </c>
       <c r="C140" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -5479,7 +5482,7 @@
         <v>142</v>
       </c>
       <c r="C142" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -5490,7 +5493,7 @@
         <v>143</v>
       </c>
       <c r="C143" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -5501,7 +5504,7 @@
         <v>144</v>
       </c>
       <c r="C144" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -5523,7 +5526,7 @@
         <v>146</v>
       </c>
       <c r="C146" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -5534,7 +5537,7 @@
         <v>147</v>
       </c>
       <c r="C147" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -5545,7 +5548,7 @@
         <v>148</v>
       </c>
       <c r="C148" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -5567,7 +5570,7 @@
         <v>150</v>
       </c>
       <c r="C150" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -5578,7 +5581,7 @@
         <v>151</v>
       </c>
       <c r="C151" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -5600,7 +5603,7 @@
         <v>153</v>
       </c>
       <c r="C153" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -5611,7 +5614,7 @@
         <v>154</v>
       </c>
       <c r="C154" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -5633,7 +5636,7 @@
         <v>156</v>
       </c>
       <c r="C156" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -5644,7 +5647,7 @@
         <v>157</v>
       </c>
       <c r="C157" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -5655,7 +5658,7 @@
         <v>158</v>
       </c>
       <c r="C158" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -5677,7 +5680,7 @@
         <v>160</v>
       </c>
       <c r="C160" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -5688,7 +5691,7 @@
         <v>161</v>
       </c>
       <c r="C161" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -5710,7 +5713,7 @@
         <v>163</v>
       </c>
       <c r="C163" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -5721,7 +5724,7 @@
         <v>164</v>
       </c>
       <c r="C164" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -5732,7 +5735,7 @@
         <v>165</v>
       </c>
       <c r="C165" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -5754,7 +5757,7 @@
         <v>167</v>
       </c>
       <c r="C167" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -5765,7 +5768,7 @@
         <v>168</v>
       </c>
       <c r="C168" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -5787,7 +5790,7 @@
         <v>170</v>
       </c>
       <c r="C170" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -5798,7 +5801,7 @@
         <v>171</v>
       </c>
       <c r="C171" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -5809,7 +5812,7 @@
         <v>172</v>
       </c>
       <c r="C172" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -5831,7 +5834,7 @@
         <v>174</v>
       </c>
       <c r="C174" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -5842,7 +5845,7 @@
         <v>175</v>
       </c>
       <c r="C175" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -5864,7 +5867,7 @@
         <v>177</v>
       </c>
       <c r="C177" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -5875,7 +5878,7 @@
         <v>178</v>
       </c>
       <c r="C178" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -5886,7 +5889,7 @@
         <v>179</v>
       </c>
       <c r="C179" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -5908,7 +5911,7 @@
         <v>181</v>
       </c>
       <c r="C181" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -5919,7 +5922,7 @@
         <v>182</v>
       </c>
       <c r="C182" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -5941,7 +5944,7 @@
         <v>184</v>
       </c>
       <c r="C184" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -5952,7 +5955,7 @@
         <v>185</v>
       </c>
       <c r="C185" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -5963,7 +5966,7 @@
         <v>186</v>
       </c>
       <c r="C186" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -5985,7 +5988,7 @@
         <v>188</v>
       </c>
       <c r="C188" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -5996,7 +5999,7 @@
         <v>189</v>
       </c>
       <c r="C189" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -6007,7 +6010,7 @@
         <v>190</v>
       </c>
       <c r="C190" t="s">
-        <v>858</v>
+        <v>831</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -6040,7 +6043,7 @@
         <v>193</v>
       </c>
       <c r="C193" t="s">
-        <v>833</v>
+        <v>860</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -6062,7 +6065,7 @@
         <v>195</v>
       </c>
       <c r="C195" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -6073,7 +6076,7 @@
         <v>196</v>
       </c>
       <c r="C196" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -6095,7 +6098,7 @@
         <v>198</v>
       </c>
       <c r="C198" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -6106,7 +6109,7 @@
         <v>199</v>
       </c>
       <c r="C199" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -6117,7 +6120,7 @@
         <v>200</v>
       </c>
       <c r="C200" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -6139,7 +6142,7 @@
         <v>202</v>
       </c>
       <c r="C202" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -6150,7 +6153,7 @@
         <v>203</v>
       </c>
       <c r="C203" t="s">
-        <v>867</v>
+        <v>854</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -6161,7 +6164,7 @@
         <v>204</v>
       </c>
       <c r="C204" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -6172,7 +6175,7 @@
         <v>205</v>
       </c>
       <c r="C205" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -6183,7 +6186,7 @@
         <v>206</v>
       </c>
       <c r="C206" t="s">
-        <v>856</v>
+        <v>867</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -6194,7 +6197,7 @@
         <v>207</v>
       </c>
       <c r="C207" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -6216,7 +6219,7 @@
         <v>209</v>
       </c>
       <c r="C209" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -6227,7 +6230,7 @@
         <v>210</v>
       </c>
       <c r="C210" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -6249,7 +6252,7 @@
         <v>212</v>
       </c>
       <c r="C212" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -6260,7 +6263,7 @@
         <v>213</v>
       </c>
       <c r="C213" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -6271,7 +6274,7 @@
         <v>214</v>
       </c>
       <c r="C214" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -6293,7 +6296,7 @@
         <v>216</v>
       </c>
       <c r="C216" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -6304,7 +6307,7 @@
         <v>217</v>
       </c>
       <c r="C217" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -6326,7 +6329,7 @@
         <v>219</v>
       </c>
       <c r="C219" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -6337,7 +6340,7 @@
         <v>220</v>
       </c>
       <c r="C220" t="s">
-        <v>876</v>
+        <v>817</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -6359,7 +6362,7 @@
         <v>222</v>
       </c>
       <c r="C222" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -6370,7 +6373,7 @@
         <v>223</v>
       </c>
       <c r="C223" t="s">
-        <v>819</v>
+        <v>877</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -6381,7 +6384,7 @@
         <v>224</v>
       </c>
       <c r="C224" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -6403,7 +6406,7 @@
         <v>226</v>
       </c>
       <c r="C226" t="s">
-        <v>879</v>
+        <v>827</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -6414,7 +6417,7 @@
         <v>227</v>
       </c>
       <c r="C227" t="s">
-        <v>880</v>
+        <v>826</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -6425,7 +6428,7 @@
         <v>228</v>
       </c>
       <c r="C228" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -6436,7 +6439,7 @@
         <v>229</v>
       </c>
       <c r="C229" t="s">
-        <v>829</v>
+        <v>880</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -6447,7 +6450,7 @@
         <v>230</v>
       </c>
       <c r="C230" t="s">
-        <v>828</v>
+        <v>880</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -6458,7 +6461,7 @@
         <v>231</v>
       </c>
       <c r="C231" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -6480,7 +6483,7 @@
         <v>233</v>
       </c>
       <c r="C233" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -6491,7 +6494,7 @@
         <v>234</v>
       </c>
       <c r="C234" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -6502,7 +6505,7 @@
         <v>235</v>
       </c>
       <c r="C235" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -6524,7 +6527,7 @@
         <v>237</v>
       </c>
       <c r="C237" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -6535,7 +6538,7 @@
         <v>238</v>
       </c>
       <c r="C238" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -6557,7 +6560,7 @@
         <v>240</v>
       </c>
       <c r="C240" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -6568,7 +6571,7 @@
         <v>241</v>
       </c>
       <c r="C241" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -6579,7 +6582,7 @@
         <v>242</v>
       </c>
       <c r="C242" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -6601,7 +6604,7 @@
         <v>244</v>
       </c>
       <c r="C244" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -6612,7 +6615,7 @@
         <v>245</v>
       </c>
       <c r="C245" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -6634,7 +6637,7 @@
         <v>247</v>
       </c>
       <c r="C247" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -6645,7 +6648,7 @@
         <v>248</v>
       </c>
       <c r="C248" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -6656,7 +6659,7 @@
         <v>249</v>
       </c>
       <c r="C249" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -6678,7 +6681,7 @@
         <v>251</v>
       </c>
       <c r="C251" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -6689,7 +6692,7 @@
         <v>252</v>
       </c>
       <c r="C252" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -6711,7 +6714,7 @@
         <v>254</v>
       </c>
       <c r="C254" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -6722,7 +6725,7 @@
         <v>255</v>
       </c>
       <c r="C255" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -6733,7 +6736,7 @@
         <v>256</v>
       </c>
       <c r="C256" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -6755,7 +6758,7 @@
         <v>258</v>
       </c>
       <c r="C258" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -6766,7 +6769,7 @@
         <v>259</v>
       </c>
       <c r="C259" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -6788,7 +6791,7 @@
         <v>261</v>
       </c>
       <c r="C261" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -6799,7 +6802,7 @@
         <v>262</v>
       </c>
       <c r="C262" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -6810,7 +6813,7 @@
         <v>263</v>
       </c>
       <c r="C263" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -6832,7 +6835,7 @@
         <v>265</v>
       </c>
       <c r="C265" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -6843,7 +6846,7 @@
         <v>266</v>
       </c>
       <c r="C266" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -6854,7 +6857,7 @@
         <v>267</v>
       </c>
       <c r="C267" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -6865,7 +6868,7 @@
         <v>268</v>
       </c>
       <c r="C268" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -6887,7 +6890,7 @@
         <v>270</v>
       </c>
       <c r="C270" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -6909,7 +6912,7 @@
         <v>272</v>
       </c>
       <c r="C272" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -6920,7 +6923,7 @@
         <v>273</v>
       </c>
       <c r="C273" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="274" spans="1:3">
@@ -6931,7 +6934,7 @@
         <v>274</v>
       </c>
       <c r="C274" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -6953,7 +6956,7 @@
         <v>276</v>
       </c>
       <c r="C276" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -6964,7 +6967,7 @@
         <v>277</v>
       </c>
       <c r="C277" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="278" spans="1:3">
@@ -6986,7 +6989,7 @@
         <v>279</v>
       </c>
       <c r="C279" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -6997,7 +7000,7 @@
         <v>280</v>
       </c>
       <c r="C280" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="281" spans="1:3">
@@ -7019,7 +7022,7 @@
         <v>282</v>
       </c>
       <c r="C282" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -7030,7 +7033,7 @@
         <v>283</v>
       </c>
       <c r="C283" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
     </row>
     <row r="284" spans="1:3">
@@ -7041,7 +7044,7 @@
         <v>284</v>
       </c>
       <c r="C284" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="285" spans="1:3">
@@ -7063,7 +7066,7 @@
         <v>286</v>
       </c>
       <c r="C286" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="287" spans="1:3">
@@ -7074,7 +7077,7 @@
         <v>287</v>
       </c>
       <c r="C287" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -7096,7 +7099,7 @@
         <v>289</v>
       </c>
       <c r="C289" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
     </row>
     <row r="290" spans="1:3">
@@ -7107,7 +7110,7 @@
         <v>290</v>
       </c>
       <c r="C290" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
     </row>
     <row r="291" spans="1:3">
@@ -7118,7 +7121,7 @@
         <v>291</v>
       </c>
       <c r="C291" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
     </row>
     <row r="292" spans="1:3">
@@ -7140,7 +7143,7 @@
         <v>293</v>
       </c>
       <c r="C293" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="294" spans="1:3">
@@ -7151,7 +7154,7 @@
         <v>294</v>
       </c>
       <c r="C294" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="295" spans="1:3">
@@ -7173,7 +7176,7 @@
         <v>296</v>
       </c>
       <c r="C296" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
     </row>
     <row r="297" spans="1:3">
@@ -7184,7 +7187,7 @@
         <v>297</v>
       </c>
       <c r="C297" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
     </row>
     <row r="298" spans="1:3">
@@ -7195,7 +7198,7 @@
         <v>298</v>
       </c>
       <c r="C298" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
     </row>
     <row r="299" spans="1:3">
@@ -7217,7 +7220,7 @@
         <v>300</v>
       </c>
       <c r="C300" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="301" spans="1:3">
@@ -7228,7 +7231,7 @@
         <v>301</v>
       </c>
       <c r="C301" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="302" spans="1:3">
@@ -7250,7 +7253,7 @@
         <v>303</v>
       </c>
       <c r="C303" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
     </row>
     <row r="304" spans="1:3">
@@ -7261,7 +7264,7 @@
         <v>304</v>
       </c>
       <c r="C304" t="s">
-        <v>930</v>
+        <v>919</v>
       </c>
     </row>
     <row r="305" spans="1:3">
@@ -7283,7 +7286,7 @@
         <v>306</v>
       </c>
       <c r="C306" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="307" spans="1:3">
@@ -7294,7 +7297,7 @@
         <v>307</v>
       </c>
       <c r="C307" t="s">
-        <v>921</v>
+        <v>931</v>
       </c>
     </row>
     <row r="308" spans="1:3">
@@ -7305,7 +7308,7 @@
         <v>308</v>
       </c>
       <c r="C308" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="309" spans="1:3">
@@ -7327,7 +7330,7 @@
         <v>310</v>
       </c>
       <c r="C310" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -7338,7 +7341,7 @@
         <v>311</v>
       </c>
       <c r="C311" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="312" spans="1:3">
@@ -7349,7 +7352,7 @@
         <v>312</v>
       </c>
       <c r="C312" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="313" spans="1:3">
@@ -7371,7 +7374,7 @@
         <v>314</v>
       </c>
       <c r="C314" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="315" spans="1:3">
@@ -7382,7 +7385,7 @@
         <v>315</v>
       </c>
       <c r="C315" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="316" spans="1:3">
@@ -7404,7 +7407,7 @@
         <v>317</v>
       </c>
       <c r="C317" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="318" spans="1:3">
@@ -7415,7 +7418,7 @@
         <v>318</v>
       </c>
       <c r="C318" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
     <row r="319" spans="1:3">
@@ -7426,7 +7429,7 @@
         <v>319</v>
       </c>
       <c r="C319" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
     </row>
     <row r="320" spans="1:3">
@@ -7448,7 +7451,7 @@
         <v>321</v>
       </c>
       <c r="C321" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="322" spans="1:3">
@@ -7459,7 +7462,7 @@
         <v>322</v>
       </c>
       <c r="C322" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="323" spans="1:3">
@@ -7481,7 +7484,7 @@
         <v>324</v>
       </c>
       <c r="C324" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="325" spans="1:3">
@@ -7492,7 +7495,7 @@
         <v>325</v>
       </c>
       <c r="C325" t="s">
-        <v>944</v>
+        <v>931</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -7514,7 +7517,7 @@
         <v>327</v>
       </c>
       <c r="C327" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="328" spans="1:3">
@@ -7525,7 +7528,7 @@
         <v>328</v>
       </c>
       <c r="C328" t="s">
-        <v>933</v>
+        <v>945</v>
       </c>
     </row>
     <row r="329" spans="1:3">
@@ -7536,7 +7539,7 @@
         <v>329</v>
       </c>
       <c r="C329" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="330" spans="1:3">
@@ -7558,7 +7561,7 @@
         <v>331</v>
       </c>
       <c r="C331" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="332" spans="1:3">
@@ -7569,7 +7572,7 @@
         <v>332</v>
       </c>
       <c r="C332" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="333" spans="1:3">
@@ -7580,7 +7583,7 @@
         <v>333</v>
       </c>
       <c r="C333" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="334" spans="1:3">
@@ -7602,7 +7605,7 @@
         <v>335</v>
       </c>
       <c r="C335" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="336" spans="1:3">
@@ -7613,7 +7616,7 @@
         <v>336</v>
       </c>
       <c r="C336" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="337" spans="1:3">
@@ -7635,7 +7638,7 @@
         <v>338</v>
       </c>
       <c r="C338" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="339" spans="1:3">
@@ -7646,7 +7649,7 @@
         <v>339</v>
       </c>
       <c r="C339" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="340" spans="1:3">
@@ -7657,7 +7660,7 @@
         <v>340</v>
       </c>
       <c r="C340" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="341" spans="1:3">
@@ -7679,7 +7682,7 @@
         <v>342</v>
       </c>
       <c r="C342" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="343" spans="1:3">
@@ -7690,7 +7693,7 @@
         <v>343</v>
       </c>
       <c r="C343" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="344" spans="1:3">
@@ -7701,7 +7704,7 @@
         <v>344</v>
       </c>
       <c r="C344" t="s">
-        <v>957</v>
+        <v>936</v>
       </c>
     </row>
     <row r="345" spans="1:3">
@@ -7734,7 +7737,7 @@
         <v>347</v>
       </c>
       <c r="C347" t="s">
-        <v>938</v>
+        <v>959</v>
       </c>
     </row>
     <row r="348" spans="1:3">
@@ -7756,7 +7759,7 @@
         <v>349</v>
       </c>
       <c r="C349" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="350" spans="1:3">
@@ -7767,7 +7770,7 @@
         <v>350</v>
       </c>
       <c r="C350" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="351" spans="1:3">
@@ -7778,7 +7781,7 @@
         <v>351</v>
       </c>
       <c r="C351" t="s">
-        <v>961</v>
+        <v>952</v>
       </c>
     </row>
     <row r="352" spans="1:3">
@@ -7811,7 +7814,7 @@
         <v>354</v>
       </c>
       <c r="C354" t="s">
-        <v>954</v>
+        <v>963</v>
       </c>
     </row>
     <row r="355" spans="1:3">
@@ -7833,7 +7836,7 @@
         <v>356</v>
       </c>
       <c r="C356" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="357" spans="1:3">
@@ -7844,7 +7847,7 @@
         <v>357</v>
       </c>
       <c r="C357" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="358" spans="1:3">
@@ -7866,7 +7869,7 @@
         <v>359</v>
       </c>
       <c r="C359" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="360" spans="1:3">
@@ -7877,7 +7880,7 @@
         <v>360</v>
       </c>
       <c r="C360" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="361" spans="1:3">
@@ -7888,7 +7891,7 @@
         <v>361</v>
       </c>
       <c r="C361" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="362" spans="1:3">
@@ -7910,7 +7913,7 @@
         <v>363</v>
       </c>
       <c r="C363" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="364" spans="1:3">
@@ -7921,7 +7924,7 @@
         <v>364</v>
       </c>
       <c r="C364" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="365" spans="1:3">
@@ -7943,7 +7946,7 @@
         <v>366</v>
       </c>
       <c r="C366" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="367" spans="1:3">
@@ -7954,7 +7957,7 @@
         <v>367</v>
       </c>
       <c r="C367" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="368" spans="1:3">
@@ -7976,7 +7979,7 @@
         <v>369</v>
       </c>
       <c r="C369" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="370" spans="1:3">
@@ -7987,7 +7990,7 @@
         <v>370</v>
       </c>
       <c r="C370" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="371" spans="1:3">
@@ -7998,7 +8001,7 @@
         <v>371</v>
       </c>
       <c r="C371" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="372" spans="1:3">
@@ -8009,7 +8012,7 @@
         <v>372</v>
       </c>
       <c r="C372" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="373" spans="1:3">
@@ -8031,7 +8034,7 @@
         <v>374</v>
       </c>
       <c r="C374" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="375" spans="1:3">
@@ -8042,7 +8045,7 @@
         <v>375</v>
       </c>
       <c r="C375" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="376" spans="1:3">
@@ -8064,7 +8067,7 @@
         <v>377</v>
       </c>
       <c r="C377" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="378" spans="1:3">
@@ -8075,7 +8078,7 @@
         <v>378</v>
       </c>
       <c r="C378" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="379" spans="1:3">
@@ -8086,7 +8089,7 @@
         <v>379</v>
       </c>
       <c r="C379" t="s">
-        <v>978</v>
+        <v>969</v>
       </c>
     </row>
     <row r="380" spans="1:3">
@@ -8097,7 +8100,7 @@
         <v>380</v>
       </c>
       <c r="C380" t="s">
-        <v>978</v>
+        <v>779</v>
       </c>
     </row>
     <row r="381" spans="1:3">
@@ -8108,7 +8111,7 @@
         <v>381</v>
       </c>
       <c r="C381" t="s">
-        <v>979</v>
+        <v>779</v>
       </c>
     </row>
     <row r="382" spans="1:3">
@@ -8119,7 +8122,7 @@
         <v>382</v>
       </c>
       <c r="C382" t="s">
-        <v>971</v>
+        <v>978</v>
       </c>
     </row>
     <row r="383" spans="1:3">
@@ -8130,7 +8133,7 @@
         <v>383</v>
       </c>
       <c r="C383" t="s">
-        <v>781</v>
+        <v>978</v>
       </c>
     </row>
     <row r="384" spans="1:3">
@@ -8141,7 +8144,7 @@
         <v>384</v>
       </c>
       <c r="C384" t="s">
-        <v>781</v>
+        <v>978</v>
       </c>
     </row>
     <row r="385" spans="1:3">
@@ -8152,7 +8155,7 @@
         <v>385</v>
       </c>
       <c r="C385" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="386" spans="1:3">
@@ -8174,7 +8177,7 @@
         <v>387</v>
       </c>
       <c r="C387" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -8185,7 +8188,7 @@
         <v>388</v>
       </c>
       <c r="C388" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="389" spans="1:3">
@@ -8196,7 +8199,7 @@
         <v>389</v>
       </c>
       <c r="C389" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="390" spans="1:3">
@@ -8218,7 +8221,7 @@
         <v>391</v>
       </c>
       <c r="C391" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="392" spans="1:3">
@@ -8229,7 +8232,7 @@
         <v>392</v>
       </c>
       <c r="C392" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="393" spans="1:3">
@@ -8240,7 +8243,7 @@
         <v>393</v>
       </c>
       <c r="C393" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="394" spans="1:3">
@@ -8262,7 +8265,7 @@
         <v>395</v>
       </c>
       <c r="C395" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="396" spans="1:3">
@@ -8273,7 +8276,7 @@
         <v>396</v>
       </c>
       <c r="C396" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="397" spans="1:3">
@@ -8295,7 +8298,7 @@
         <v>398</v>
       </c>
       <c r="C398" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="399" spans="1:3">
@@ -8306,7 +8309,7 @@
         <v>399</v>
       </c>
       <c r="C399" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="400" spans="1:3">
@@ -8317,7 +8320,7 @@
         <v>400</v>
       </c>
       <c r="C400" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="401" spans="1:3">
@@ -8339,7 +8342,7 @@
         <v>402</v>
       </c>
       <c r="C402" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="403" spans="1:3">
@@ -8350,7 +8353,7 @@
         <v>403</v>
       </c>
       <c r="C403" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="404" spans="1:3">
@@ -8372,7 +8375,7 @@
         <v>405</v>
       </c>
       <c r="C405" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="406" spans="1:3">
@@ -8383,7 +8386,7 @@
         <v>406</v>
       </c>
       <c r="C406" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="407" spans="1:3">
@@ -8405,7 +8408,7 @@
         <v>408</v>
       </c>
       <c r="C408" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="409" spans="1:3">
@@ -8416,7 +8419,7 @@
         <v>409</v>
       </c>
       <c r="C409" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="410" spans="1:3">
@@ -8427,7 +8430,7 @@
         <v>410</v>
       </c>
       <c r="C410" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="411" spans="1:3">
@@ -8449,7 +8452,7 @@
         <v>412</v>
       </c>
       <c r="C412" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="413" spans="1:3">
@@ -8460,7 +8463,7 @@
         <v>413</v>
       </c>
       <c r="C413" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="414" spans="1:3">
@@ -8482,7 +8485,7 @@
         <v>415</v>
       </c>
       <c r="C415" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="416" spans="1:3">
@@ -8493,7 +8496,7 @@
         <v>416</v>
       </c>
       <c r="C416" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="417" spans="1:3">
@@ -8504,7 +8507,7 @@
         <v>417</v>
       </c>
       <c r="C417" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="418" spans="1:3">
@@ -8526,7 +8529,7 @@
         <v>419</v>
       </c>
       <c r="C419" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="420" spans="1:3">
@@ -8537,7 +8540,7 @@
         <v>420</v>
       </c>
       <c r="C420" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="421" spans="1:3">
@@ -8548,7 +8551,7 @@
         <v>421</v>
       </c>
       <c r="C421" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="422" spans="1:3">
@@ -8570,7 +8573,7 @@
         <v>423</v>
       </c>
       <c r="C423" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="424" spans="1:3">
@@ -8581,7 +8584,7 @@
         <v>424</v>
       </c>
       <c r="C424" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="425" spans="1:3">
@@ -8603,7 +8606,7 @@
         <v>426</v>
       </c>
       <c r="C426" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="427" spans="1:3">
@@ -8614,7 +8617,7 @@
         <v>427</v>
       </c>
       <c r="C427" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="428" spans="1:3">
@@ -8636,7 +8639,7 @@
         <v>429</v>
       </c>
       <c r="C429" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="430" spans="1:3">
@@ -8647,7 +8650,7 @@
         <v>430</v>
       </c>
       <c r="C430" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="431" spans="1:3">
@@ -8658,7 +8661,7 @@
         <v>431</v>
       </c>
       <c r="C431" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="432" spans="1:3">
@@ -8680,7 +8683,7 @@
         <v>433</v>
       </c>
       <c r="C433" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="434" spans="1:3">
@@ -8691,7 +8694,7 @@
         <v>434</v>
       </c>
       <c r="C434" t="s">
-        <v>1012</v>
+        <v>992</v>
       </c>
     </row>
     <row r="435" spans="1:3">
@@ -8702,7 +8705,7 @@
         <v>435</v>
       </c>
       <c r="C435" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="436" spans="1:3">
@@ -8724,7 +8727,7 @@
         <v>437</v>
       </c>
       <c r="C437" t="s">
-        <v>994</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="438" spans="1:3">
@@ -8735,7 +8738,7 @@
         <v>438</v>
       </c>
       <c r="C438" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="439" spans="1:3">
@@ -8757,7 +8760,7 @@
         <v>440</v>
       </c>
       <c r="C440" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="441" spans="1:3">
@@ -8768,7 +8771,7 @@
         <v>441</v>
       </c>
       <c r="C441" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="442" spans="1:3">
@@ -8790,7 +8793,7 @@
         <v>443</v>
       </c>
       <c r="C443" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="444" spans="1:3">
@@ -8801,7 +8804,7 @@
         <v>444</v>
       </c>
       <c r="C444" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="445" spans="1:3">
@@ -8812,7 +8815,7 @@
         <v>445</v>
       </c>
       <c r="C445" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="446" spans="1:3">
@@ -8823,7 +8826,7 @@
         <v>446</v>
       </c>
       <c r="C446" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="447" spans="1:3">
@@ -8834,7 +8837,7 @@
         <v>447</v>
       </c>
       <c r="C447" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="448" spans="1:3">
@@ -8856,7 +8859,7 @@
         <v>449</v>
       </c>
       <c r="C449" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="450" spans="1:3">
@@ -8867,7 +8870,7 @@
         <v>450</v>
       </c>
       <c r="C450" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="451" spans="1:3">
@@ -8878,7 +8881,7 @@
         <v>451</v>
       </c>
       <c r="C451" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="452" spans="1:3">
@@ -8889,7 +8892,7 @@
         <v>452</v>
       </c>
       <c r="C452" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="453" spans="1:3">
@@ -8911,7 +8914,7 @@
         <v>454</v>
       </c>
       <c r="C454" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="455" spans="1:3">
@@ -8922,7 +8925,7 @@
         <v>455</v>
       </c>
       <c r="C455" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="456" spans="1:3">
@@ -8944,7 +8947,7 @@
         <v>457</v>
       </c>
       <c r="C457" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="458" spans="1:3">
@@ -8955,7 +8958,7 @@
         <v>458</v>
       </c>
       <c r="C458" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="459" spans="1:3">
@@ -8966,7 +8969,7 @@
         <v>459</v>
       </c>
       <c r="C459" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="460" spans="1:3">
@@ -8988,7 +8991,7 @@
         <v>461</v>
       </c>
       <c r="C461" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="462" spans="1:3">
@@ -8999,7 +9002,7 @@
         <v>462</v>
       </c>
       <c r="C462" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="463" spans="1:3">
@@ -9021,7 +9024,7 @@
         <v>464</v>
       </c>
       <c r="C464" t="s">
-        <v>1030</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="465" spans="1:3">
@@ -9043,7 +9046,7 @@
         <v>466</v>
       </c>
       <c r="C466" t="s">
-        <v>1032</v>
+        <v>956</v>
       </c>
     </row>
     <row r="467" spans="1:3">
@@ -9054,7 +9057,7 @@
         <v>467</v>
       </c>
       <c r="C467" t="s">
-        <v>1022</v>
+        <v>956</v>
       </c>
     </row>
     <row r="468" spans="1:3">
@@ -9065,7 +9068,7 @@
         <v>468</v>
       </c>
       <c r="C468" t="s">
-        <v>1033</v>
+        <v>956</v>
       </c>
     </row>
     <row r="469" spans="1:3">
@@ -9076,7 +9079,7 @@
         <v>469</v>
       </c>
       <c r="C469" t="s">
-        <v>958</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="470" spans="1:3">
@@ -9087,7 +9090,7 @@
         <v>470</v>
       </c>
       <c r="C470" t="s">
-        <v>958</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="471" spans="1:3">
@@ -9098,7 +9101,7 @@
         <v>471</v>
       </c>
       <c r="C471" t="s">
-        <v>958</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="472" spans="1:3">
@@ -9109,7 +9112,7 @@
         <v>472</v>
       </c>
       <c r="C472" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="473" spans="1:3">
@@ -9120,7 +9123,7 @@
         <v>473</v>
       </c>
       <c r="C473" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="474" spans="1:3">
@@ -9142,7 +9145,7 @@
         <v>475</v>
       </c>
       <c r="C475" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="476" spans="1:3">
@@ -9153,7 +9156,7 @@
         <v>476</v>
       </c>
       <c r="C476" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="477" spans="1:3">
@@ -9175,7 +9178,7 @@
         <v>478</v>
       </c>
       <c r="C478" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="479" spans="1:3">
@@ -9186,7 +9189,7 @@
         <v>479</v>
       </c>
       <c r="C479" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="480" spans="1:3">
@@ -9197,7 +9200,7 @@
         <v>480</v>
       </c>
       <c r="C480" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="481" spans="1:3">
@@ -9219,7 +9222,7 @@
         <v>482</v>
       </c>
       <c r="C482" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="483" spans="1:3">
@@ -9230,7 +9233,7 @@
         <v>483</v>
       </c>
       <c r="C483" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="484" spans="1:3">
@@ -9252,7 +9255,7 @@
         <v>485</v>
       </c>
       <c r="C485" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="486" spans="1:3">
@@ -9263,7 +9266,7 @@
         <v>486</v>
       </c>
       <c r="C486" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="487" spans="1:3">
@@ -9274,7 +9277,7 @@
         <v>487</v>
       </c>
       <c r="C487" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="488" spans="1:3">
@@ -9296,7 +9299,7 @@
         <v>489</v>
       </c>
       <c r="C489" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="490" spans="1:3">
@@ -9307,7 +9310,7 @@
         <v>490</v>
       </c>
       <c r="C490" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="491" spans="1:3">
@@ -9329,7 +9332,7 @@
         <v>492</v>
       </c>
       <c r="C492" t="s">
-        <v>1048</v>
+        <v>907</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -9362,7 +9365,7 @@
         <v>495</v>
       </c>
       <c r="C495" t="s">
-        <v>909</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -9373,7 +9376,7 @@
         <v>496</v>
       </c>
       <c r="C496" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="497" spans="1:3">
@@ -9384,7 +9387,7 @@
         <v>497</v>
       </c>
       <c r="C497" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="498" spans="1:3">
@@ -9395,7 +9398,7 @@
         <v>498</v>
       </c>
       <c r="C498" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="499" spans="1:3">
@@ -9417,7 +9420,7 @@
         <v>500</v>
       </c>
       <c r="C500" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="501" spans="1:3">
@@ -9428,7 +9431,7 @@
         <v>501</v>
       </c>
       <c r="C501" t="s">
-        <v>1053</v>
+        <v>994</v>
       </c>
     </row>
     <row r="502" spans="1:3">
@@ -9439,7 +9442,7 @@
         <v>502</v>
       </c>
       <c r="C502" t="s">
-        <v>1054</v>
+        <v>994</v>
       </c>
     </row>
     <row r="503" spans="1:3">
@@ -9450,7 +9453,7 @@
         <v>503</v>
       </c>
       <c r="C503" t="s">
-        <v>1055</v>
+        <v>994</v>
       </c>
     </row>
     <row r="504" spans="1:3">
@@ -9461,7 +9464,7 @@
         <v>504</v>
       </c>
       <c r="C504" t="s">
-        <v>996</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="505" spans="1:3">
@@ -9472,7 +9475,7 @@
         <v>505</v>
       </c>
       <c r="C505" t="s">
-        <v>996</v>
+        <v>890</v>
       </c>
     </row>
     <row r="506" spans="1:3">
@@ -9483,7 +9486,7 @@
         <v>506</v>
       </c>
       <c r="C506" t="s">
-        <v>996</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="507" spans="1:3">
@@ -9505,7 +9508,7 @@
         <v>508</v>
       </c>
       <c r="C508" t="s">
-        <v>892</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="509" spans="1:3">
@@ -9527,7 +9530,7 @@
         <v>510</v>
       </c>
       <c r="C510" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="511" spans="1:3">
@@ -9538,7 +9541,7 @@
         <v>511</v>
       </c>
       <c r="C511" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -9549,7 +9552,7 @@
         <v>512</v>
       </c>
       <c r="C512" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="513" spans="1:3">
@@ -9571,7 +9574,7 @@
         <v>514</v>
       </c>
       <c r="C514" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="515" spans="1:3">
@@ -9582,7 +9585,7 @@
         <v>515</v>
       </c>
       <c r="C515" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="516" spans="1:3">
@@ -9604,7 +9607,7 @@
         <v>517</v>
       </c>
       <c r="C517" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="518" spans="1:3">
@@ -9615,7 +9618,7 @@
         <v>518</v>
       </c>
       <c r="C518" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="519" spans="1:3">
@@ -9626,7 +9629,7 @@
         <v>519</v>
       </c>
       <c r="C519" t="s">
-        <v>1063</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="520" spans="1:3">
@@ -9637,7 +9640,7 @@
         <v>520</v>
       </c>
       <c r="C520" t="s">
-        <v>1063</v>
+        <v>907</v>
       </c>
     </row>
     <row r="521" spans="1:3">
@@ -9648,7 +9651,7 @@
         <v>521</v>
       </c>
       <c r="C521" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="522" spans="1:3">
@@ -9659,7 +9662,7 @@
         <v>522</v>
       </c>
       <c r="C522" t="s">
-        <v>1039</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="523" spans="1:3">
@@ -9670,7 +9673,7 @@
         <v>523</v>
       </c>
       <c r="C523" t="s">
-        <v>909</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="524" spans="1:3">
@@ -9681,7 +9684,7 @@
         <v>524</v>
       </c>
       <c r="C524" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="525" spans="1:3">
@@ -9692,7 +9695,7 @@
         <v>525</v>
       </c>
       <c r="C525" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="526" spans="1:3">
@@ -9714,7 +9717,7 @@
         <v>527</v>
       </c>
       <c r="C527" t="s">
-        <v>1066</v>
+        <v>784</v>
       </c>
     </row>
     <row r="528" spans="1:3">
@@ -9747,7 +9750,7 @@
         <v>530</v>
       </c>
       <c r="C530" t="s">
-        <v>786</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="531" spans="1:3">
@@ -9758,7 +9761,7 @@
         <v>531</v>
       </c>
       <c r="C531" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="532" spans="1:3">
@@ -9769,7 +9772,7 @@
         <v>532</v>
       </c>
       <c r="C532" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="533" spans="1:3">
@@ -9791,7 +9794,7 @@
         <v>534</v>
       </c>
       <c r="C534" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="535" spans="1:3">
@@ -9802,7 +9805,7 @@
         <v>535</v>
       </c>
       <c r="C535" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="536" spans="1:3">
@@ -9813,7 +9816,7 @@
         <v>536</v>
       </c>
       <c r="C536" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="537" spans="1:3">
@@ -9835,7 +9838,7 @@
         <v>538</v>
       </c>
       <c r="C538" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="539" spans="1:3">
@@ -9846,7 +9849,7 @@
         <v>539</v>
       </c>
       <c r="C539" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="540" spans="1:3">
@@ -9868,7 +9871,7 @@
         <v>541</v>
       </c>
       <c r="C541" t="s">
-        <v>1075</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="542" spans="1:3">
@@ -9901,7 +9904,7 @@
         <v>544</v>
       </c>
       <c r="C544" t="s">
-        <v>1005</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="545" spans="1:3">
@@ -9912,7 +9915,7 @@
         <v>545</v>
       </c>
       <c r="C545" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="546" spans="1:3">
@@ -9923,7 +9926,7 @@
         <v>546</v>
       </c>
       <c r="C546" t="s">
-        <v>1079</v>
+        <v>824</v>
       </c>
     </row>
     <row r="547" spans="1:3">
@@ -9934,7 +9937,7 @@
         <v>547</v>
       </c>
       <c r="C547" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="548" spans="1:3">
@@ -9945,7 +9948,7 @@
         <v>548</v>
       </c>
       <c r="C548" t="s">
-        <v>1079</v>
+        <v>828</v>
       </c>
     </row>
     <row r="549" spans="1:3">
@@ -9956,7 +9959,7 @@
         <v>549</v>
       </c>
       <c r="C549" t="s">
-        <v>826</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="550" spans="1:3">
@@ -9978,7 +9981,7 @@
         <v>551</v>
       </c>
       <c r="C551" t="s">
-        <v>830</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="552" spans="1:3">
@@ -9989,7 +9992,7 @@
         <v>552</v>
       </c>
       <c r="C552" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="553" spans="1:3">
@@ -10000,7 +10003,7 @@
         <v>553</v>
       </c>
       <c r="C553" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="554" spans="1:3">
@@ -10022,7 +10025,7 @@
         <v>555</v>
       </c>
       <c r="C555" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="556" spans="1:3">
@@ -10033,7 +10036,7 @@
         <v>556</v>
       </c>
       <c r="C556" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="557" spans="1:3">
@@ -10044,7 +10047,7 @@
         <v>557</v>
       </c>
       <c r="C557" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="558" spans="1:3">
@@ -10066,7 +10069,7 @@
         <v>559</v>
       </c>
       <c r="C559" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="560" spans="1:3">
@@ -10077,7 +10080,7 @@
         <v>560</v>
       </c>
       <c r="C560" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="561" spans="1:3">
@@ -10099,7 +10102,7 @@
         <v>562</v>
       </c>
       <c r="C562" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="563" spans="1:3">
@@ -10110,7 +10113,7 @@
         <v>563</v>
       </c>
       <c r="C563" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="564" spans="1:3">
@@ -10121,7 +10124,7 @@
         <v>564</v>
       </c>
       <c r="C564" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="565" spans="1:3">
@@ -10143,7 +10146,7 @@
         <v>566</v>
       </c>
       <c r="C566" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="567" spans="1:3">
@@ -10154,7 +10157,7 @@
         <v>567</v>
       </c>
       <c r="C567" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="568" spans="1:3">
@@ -10165,7 +10168,7 @@
         <v>568</v>
       </c>
       <c r="C568" t="s">
-        <v>1092</v>
+        <v>881</v>
       </c>
     </row>
     <row r="569" spans="1:3">
@@ -10198,7 +10201,7 @@
         <v>571</v>
       </c>
       <c r="C571" t="s">
-        <v>883</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="572" spans="1:3">
@@ -10220,7 +10223,7 @@
         <v>573</v>
       </c>
       <c r="C573" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="574" spans="1:3">
@@ -10231,7 +10234,7 @@
         <v>574</v>
       </c>
       <c r="C574" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="575" spans="1:3">
@@ -10253,7 +10256,7 @@
         <v>576</v>
       </c>
       <c r="C576" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="577" spans="1:3">
@@ -10264,7 +10267,7 @@
         <v>577</v>
       </c>
       <c r="C577" t="s">
-        <v>1097</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="578" spans="1:3">
@@ -10275,7 +10278,7 @@
         <v>578</v>
       </c>
       <c r="C578" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="579" spans="1:3">
@@ -10297,7 +10300,7 @@
         <v>580</v>
       </c>
       <c r="C580" t="s">
-        <v>1077</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="581" spans="1:3">
@@ -10308,7 +10311,7 @@
         <v>581</v>
       </c>
       <c r="C581" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="582" spans="1:3">
@@ -10330,7 +10333,7 @@
         <v>583</v>
       </c>
       <c r="C583" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="584" spans="1:3">
@@ -10341,7 +10344,7 @@
         <v>584</v>
       </c>
       <c r="C584" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="585" spans="1:3">
@@ -10352,7 +10355,7 @@
         <v>585</v>
       </c>
       <c r="C585" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="586" spans="1:3">
@@ -10374,7 +10377,7 @@
         <v>587</v>
       </c>
       <c r="C587" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="588" spans="1:3">
@@ -10385,7 +10388,7 @@
         <v>588</v>
       </c>
       <c r="C588" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="589" spans="1:3">
@@ -10407,7 +10410,7 @@
         <v>590</v>
       </c>
       <c r="C590" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="591" spans="1:3">
@@ -10418,7 +10421,7 @@
         <v>591</v>
       </c>
       <c r="C591" t="s">
-        <v>1105</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="592" spans="1:3">
@@ -10440,7 +10443,7 @@
         <v>593</v>
       </c>
       <c r="C593" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="594" spans="1:3">
@@ -10451,7 +10454,7 @@
         <v>594</v>
       </c>
       <c r="C594" t="s">
-        <v>1024</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="595" spans="1:3">
@@ -10462,7 +10465,7 @@
         <v>595</v>
       </c>
       <c r="C595" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="596" spans="1:3">
@@ -10484,7 +10487,7 @@
         <v>597</v>
       </c>
       <c r="C597" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="598" spans="1:3">
@@ -10495,7 +10498,7 @@
         <v>598</v>
       </c>
       <c r="C598" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="599" spans="1:3">
@@ -10506,7 +10509,7 @@
         <v>599</v>
       </c>
       <c r="C599" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="600" spans="1:3">
@@ -10528,7 +10531,7 @@
         <v>601</v>
       </c>
       <c r="C601" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="602" spans="1:3">
@@ -10539,7 +10542,7 @@
         <v>602</v>
       </c>
       <c r="C602" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="603" spans="1:3">
@@ -10561,7 +10564,7 @@
         <v>604</v>
       </c>
       <c r="C604" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="605" spans="1:3">
@@ -10572,7 +10575,7 @@
         <v>605</v>
       </c>
       <c r="C605" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="606" spans="1:3">
@@ -10583,7 +10586,7 @@
         <v>606</v>
       </c>
       <c r="C606" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="607" spans="1:3">
@@ -10605,7 +10608,7 @@
         <v>608</v>
       </c>
       <c r="C608" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="609" spans="1:3">
@@ -10616,7 +10619,7 @@
         <v>609</v>
       </c>
       <c r="C609" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="610" spans="1:3">
@@ -10638,7 +10641,7 @@
         <v>611</v>
       </c>
       <c r="C611" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="612" spans="1:3">
@@ -10649,7 +10652,7 @@
         <v>612</v>
       </c>
       <c r="C612" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="613" spans="1:3">
@@ -10660,7 +10663,7 @@
         <v>613</v>
       </c>
       <c r="C613" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="614" spans="1:3">
@@ -10682,7 +10685,7 @@
         <v>615</v>
       </c>
       <c r="C615" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="616" spans="1:3">
@@ -10693,7 +10696,7 @@
         <v>616</v>
       </c>
       <c r="C616" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="617" spans="1:3">
@@ -10715,7 +10718,7 @@
         <v>618</v>
       </c>
       <c r="C618" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="619" spans="1:3">
@@ -10726,7 +10729,7 @@
         <v>619</v>
       </c>
       <c r="C619" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="620" spans="1:3">
@@ -10737,7 +10740,7 @@
         <v>620</v>
       </c>
       <c r="C620" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="621" spans="1:3">
@@ -10759,7 +10762,7 @@
         <v>622</v>
       </c>
       <c r="C622" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="623" spans="1:3">
@@ -10770,7 +10773,7 @@
         <v>623</v>
       </c>
       <c r="C623" t="s">
-        <v>1128</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="624" spans="1:3">
@@ -10781,7 +10784,7 @@
         <v>624</v>
       </c>
       <c r="C624" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="625" spans="1:3">
@@ -10803,7 +10806,7 @@
         <v>626</v>
       </c>
       <c r="C626" t="s">
-        <v>1069</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="627" spans="1:3">
@@ -10814,7 +10817,7 @@
         <v>627</v>
       </c>
       <c r="C627" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="628" spans="1:3">
@@ -10836,7 +10839,7 @@
         <v>629</v>
       </c>
       <c r="C629" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="630" spans="1:3">
@@ -10847,7 +10850,7 @@
         <v>630</v>
       </c>
       <c r="C630" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="631" spans="1:3">
@@ -10858,7 +10861,7 @@
         <v>631</v>
       </c>
       <c r="C631" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="632" spans="1:3">
@@ -10869,7 +10872,7 @@
         <v>632</v>
       </c>
       <c r="C632" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="633" spans="1:3">
@@ -10891,7 +10894,7 @@
         <v>634</v>
       </c>
       <c r="C634" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="635" spans="1:3">
@@ -10913,7 +10916,7 @@
         <v>636</v>
       </c>
       <c r="C636" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="637" spans="1:3">
@@ -10924,7 +10927,7 @@
         <v>637</v>
       </c>
       <c r="C637" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="638" spans="1:3">
@@ -10935,7 +10938,7 @@
         <v>638</v>
       </c>
       <c r="C638" t="s">
-        <v>1135</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="639" spans="1:3">
@@ -10946,7 +10949,7 @@
         <v>639</v>
       </c>
       <c r="C639" t="s">
-        <v>1135</v>
+        <v>897</v>
       </c>
     </row>
     <row r="640" spans="1:3">
@@ -10957,7 +10960,7 @@
         <v>640</v>
       </c>
       <c r="C640" t="s">
-        <v>1135</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="641" spans="1:3">
@@ -10968,7 +10971,7 @@
         <v>641</v>
       </c>
       <c r="C641" t="s">
-        <v>1039</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="642" spans="1:3">
@@ -10979,7 +10982,7 @@
         <v>642</v>
       </c>
       <c r="C642" t="s">
-        <v>899</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="643" spans="1:3">
@@ -10990,7 +10993,7 @@
         <v>643</v>
       </c>
       <c r="C643" t="s">
-        <v>1060</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="644" spans="1:3">
@@ -11001,7 +11004,7 @@
         <v>644</v>
       </c>
       <c r="C644" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="645" spans="1:3">
@@ -11023,7 +11026,7 @@
         <v>646</v>
       </c>
       <c r="C646" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="647" spans="1:3">
@@ -11034,7 +11037,7 @@
         <v>647</v>
       </c>
       <c r="C647" t="s">
-        <v>1137</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="648" spans="1:3">
@@ -11056,7 +11059,7 @@
         <v>649</v>
       </c>
       <c r="C649" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="650" spans="1:3">
@@ -11067,7 +11070,7 @@
         <v>650</v>
       </c>
       <c r="C650" t="s">
-        <v>1117</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="651" spans="1:3">
@@ -11078,7 +11081,7 @@
         <v>651</v>
       </c>
       <c r="C651" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="652" spans="1:3">
@@ -11089,7 +11092,7 @@
         <v>652</v>
       </c>
       <c r="C652" t="s">
-        <v>1140</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="653" spans="1:3">
@@ -11100,7 +11103,7 @@
         <v>653</v>
       </c>
       <c r="C653" t="s">
-        <v>1140</v>
+        <v>838</v>
       </c>
     </row>
     <row r="654" spans="1:3">
@@ -11111,7 +11114,7 @@
         <v>654</v>
       </c>
       <c r="C654" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="655" spans="1:3">
@@ -11122,7 +11125,7 @@
         <v>655</v>
       </c>
       <c r="C655" t="s">
-        <v>1029</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="656" spans="1:3">
@@ -11133,7 +11136,7 @@
         <v>656</v>
       </c>
       <c r="C656" t="s">
-        <v>840</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="657" spans="1:3">
@@ -11144,7 +11147,7 @@
         <v>657</v>
       </c>
       <c r="C657" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="658" spans="1:3">
@@ -11155,7 +11158,7 @@
         <v>658</v>
       </c>
       <c r="C658" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="659" spans="1:3">
@@ -11177,7 +11180,7 @@
         <v>660</v>
       </c>
       <c r="C660" t="s">
-        <v>1143</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="661" spans="1:3">
@@ -11188,7 +11191,7 @@
         <v>661</v>
       </c>
       <c r="C661" t="s">
-        <v>1144</v>
+        <v>985</v>
       </c>
     </row>
     <row r="662" spans="1:3">
@@ -11199,7 +11202,7 @@
         <v>662</v>
       </c>
       <c r="C662" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="663" spans="1:3">
@@ -11210,7 +11213,7 @@
         <v>663</v>
       </c>
       <c r="C663" t="s">
-        <v>1131</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="664" spans="1:3">
@@ -11221,7 +11224,7 @@
         <v>664</v>
       </c>
       <c r="C664" t="s">
-        <v>987</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="665" spans="1:3">
@@ -11232,7 +11235,7 @@
         <v>665</v>
       </c>
       <c r="C665" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="666" spans="1:3">
@@ -11254,7 +11257,7 @@
         <v>667</v>
       </c>
       <c r="C667" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="668" spans="1:3">
@@ -11265,7 +11268,7 @@
         <v>668</v>
       </c>
       <c r="C668" t="s">
-        <v>1147</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="669" spans="1:3">
@@ -11287,7 +11290,7 @@
         <v>670</v>
       </c>
       <c r="C670" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="671" spans="1:3">
@@ -11298,7 +11301,7 @@
         <v>671</v>
       </c>
       <c r="C671" t="s">
-        <v>1021</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="672" spans="1:3">
@@ -11309,7 +11312,7 @@
         <v>672</v>
       </c>
       <c r="C672" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="673" spans="1:3">
@@ -11320,7 +11323,7 @@
         <v>673</v>
       </c>
       <c r="C673" t="s">
-        <v>1150</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="674" spans="1:3">
@@ -11331,7 +11334,7 @@
         <v>674</v>
       </c>
       <c r="C674" t="s">
-        <v>1150</v>
+        <v>783</v>
       </c>
     </row>
     <row r="675" spans="1:3">
@@ -11342,7 +11345,7 @@
         <v>675</v>
       </c>
       <c r="C675" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="676" spans="1:3">
@@ -11353,7 +11356,7 @@
         <v>676</v>
       </c>
       <c r="C676" t="s">
-        <v>1029</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="677" spans="1:3">
@@ -11364,7 +11367,7 @@
         <v>677</v>
       </c>
       <c r="C677" t="s">
-        <v>785</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="678" spans="1:3">
@@ -11375,7 +11378,7 @@
         <v>678</v>
       </c>
       <c r="C678" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="679" spans="1:3">
@@ -11386,7 +11389,7 @@
         <v>679</v>
       </c>
       <c r="C679" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="680" spans="1:3">
@@ -11408,7 +11411,7 @@
         <v>681</v>
       </c>
       <c r="C681" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="682" spans="1:3">
@@ -11419,7 +11422,7 @@
         <v>682</v>
       </c>
       <c r="C682" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="683" spans="1:3">
@@ -11430,7 +11433,7 @@
         <v>683</v>
       </c>
       <c r="C683" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="684" spans="1:3">
@@ -11452,7 +11455,7 @@
         <v>685</v>
       </c>
       <c r="C685" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="686" spans="1:3">
@@ -11463,7 +11466,7 @@
         <v>686</v>
       </c>
       <c r="C686" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="687" spans="1:3">
@@ -11485,7 +11488,7 @@
         <v>688</v>
       </c>
       <c r="C688" t="s">
-        <v>1158</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="689" spans="1:3">
@@ -11518,7 +11521,7 @@
         <v>691</v>
       </c>
       <c r="C691" t="s">
-        <v>1047</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="692" spans="1:3">
@@ -11529,7 +11532,7 @@
         <v>692</v>
       </c>
       <c r="C692" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="693" spans="1:3">
@@ -11540,7 +11543,7 @@
         <v>693</v>
       </c>
       <c r="C693" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="694" spans="1:3">
@@ -11562,7 +11565,7 @@
         <v>695</v>
       </c>
       <c r="C695" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="696" spans="1:3">
@@ -11573,7 +11576,7 @@
         <v>696</v>
       </c>
       <c r="C696" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="697" spans="1:3">
@@ -11584,7 +11587,7 @@
         <v>697</v>
       </c>
       <c r="C697" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="698" spans="1:3">
@@ -11606,7 +11609,7 @@
         <v>699</v>
       </c>
       <c r="C699" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="700" spans="1:3">
@@ -11617,7 +11620,7 @@
         <v>700</v>
       </c>
       <c r="C700" t="s">
-        <v>1167</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="701" spans="1:3">
@@ -11628,7 +11631,7 @@
         <v>701</v>
       </c>
       <c r="C701" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="702" spans="1:3">
@@ -11639,7 +11642,7 @@
         <v>702</v>
       </c>
       <c r="C702" t="s">
-        <v>1167</v>
+        <v>877</v>
       </c>
     </row>
     <row r="703" spans="1:3">
@@ -11650,7 +11653,7 @@
         <v>703</v>
       </c>
       <c r="C703" t="s">
-        <v>1021</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="704" spans="1:3">
@@ -11672,7 +11675,7 @@
         <v>705</v>
       </c>
       <c r="C705" t="s">
-        <v>879</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="706" spans="1:3">
@@ -11683,7 +11686,7 @@
         <v>706</v>
       </c>
       <c r="C706" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="707" spans="1:3">
@@ -11694,7 +11697,7 @@
         <v>707</v>
       </c>
       <c r="C707" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="708" spans="1:3">
@@ -11716,7 +11719,7 @@
         <v>709</v>
       </c>
       <c r="C709" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="710" spans="1:3">
@@ -11727,7 +11730,7 @@
         <v>710</v>
       </c>
       <c r="C710" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="711" spans="1:3">
@@ -11738,7 +11741,7 @@
         <v>711</v>
       </c>
       <c r="C711" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="712" spans="1:3">
@@ -11760,7 +11763,7 @@
         <v>713</v>
       </c>
       <c r="C713" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="714" spans="1:3">
@@ -11771,7 +11774,7 @@
         <v>714</v>
       </c>
       <c r="C714" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="715" spans="1:3">
@@ -11782,7 +11785,7 @@
         <v>715</v>
       </c>
       <c r="C715" t="s">
-        <v>1175</v>
+        <v>779</v>
       </c>
     </row>
     <row r="716" spans="1:3">
@@ -11815,7 +11818,7 @@
         <v>718</v>
       </c>
       <c r="C718" t="s">
-        <v>781</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="719" spans="1:3">
@@ -11837,7 +11840,7 @@
         <v>720</v>
       </c>
       <c r="C720" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="721" spans="1:3">
@@ -11848,7 +11851,7 @@
         <v>721</v>
       </c>
       <c r="C721" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="722" spans="1:3">
@@ -11870,7 +11873,7 @@
         <v>723</v>
       </c>
       <c r="C723" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="724" spans="1:3">
@@ -11881,7 +11884,7 @@
         <v>724</v>
       </c>
       <c r="C724" t="s">
-        <v>1180</v>
+        <v>781</v>
       </c>
     </row>
     <row r="725" spans="1:3">
@@ -11892,7 +11895,7 @@
         <v>725</v>
       </c>
       <c r="C725" t="s">
-        <v>1181</v>
+        <v>781</v>
       </c>
     </row>
     <row r="726" spans="1:3">
@@ -11903,7 +11906,7 @@
         <v>726</v>
       </c>
       <c r="C726" t="s">
-        <v>1182</v>
+        <v>781</v>
       </c>
     </row>
     <row r="727" spans="1:3">
@@ -11914,7 +11917,7 @@
         <v>727</v>
       </c>
       <c r="C727" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="728" spans="1:3">
@@ -11925,7 +11928,7 @@
         <v>728</v>
       </c>
       <c r="C728" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="729" spans="1:3">
@@ -11936,7 +11939,7 @@
         <v>729</v>
       </c>
       <c r="C729" t="s">
-        <v>783</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="730" spans="1:3">
@@ -11947,7 +11950,7 @@
         <v>730</v>
       </c>
       <c r="C730" t="s">
-        <v>783</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="731" spans="1:3">
@@ -11958,7 +11961,7 @@
         <v>731</v>
       </c>
       <c r="C731" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
     </row>
     <row r="732" spans="1:3">
@@ -11969,7 +11972,7 @@
         <v>732</v>
       </c>
       <c r="C732" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>